<commit_message>
updated code to rpm and tnker cad design
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Arduino\december\arduino_laser_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A220EBC9-6638-4A45-AC6C-E8E2FA54D1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7004799F-C4B6-4B27-B6E2-94F86F891648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="35" uniqueCount="35">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="43" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -63,18 +63,12 @@
     <t>D1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Diode</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t>MCP23008-based, 32 LCD 16 x 2 (I2C)</t>
   </si>
   <si>
-    <t>D2, D4</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -84,27 +78,12 @@
     <t>1 kΩ Resistor</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>10 kΩ Resistor</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>100 Ω Resistor</t>
-  </si>
-  <si>
     <t>BAT1</t>
   </si>
   <si>
     <t xml:space="preserve"> 9V Battery</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NPN Transistor (BJT)</t>
   </si>
   <si>
@@ -130,12 +109,54 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/rochester-electronics-llc/2N3053/12094898</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R6</t>
+  </si>
+  <si>
+    <t>200 Ω Resistor</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Optocoupler</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pushbutton</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>LASER MODULE</t>
+  </si>
+  <si>
+    <t>1N4004</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Youliang-KY-008-Transmitter-Arduino-Raspberry/dp/B07ST98B7S/ref=sr_1_9?keywords=arduino+laser&amp;qid=1675077760&amp;sr=8-9</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/4N35-Optocouplers-Phototransistor-30V-IC/dp/B0073BOU46</t>
+  </si>
+  <si>
+    <t>https://rubikstech.co.ke/index.php?route=product/product&amp;product_id=283</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Duracell-Coppertop-Alkaline-Batteries-Count/dp/B000K2NW08?th=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -980,11 +1001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1031,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1045,7 +1066,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1070,103 +1091,137 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D676F9E2-C12C-452F-B3CE-FAF068A8B7F9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FFAB5761-4278-4797-83E2-7C945B353969}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{E394C476-06B4-4873-87DE-990E4C718E0B}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{964E911E-D539-4718-B64A-704B98CD1A5E}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{A11DA3AB-5147-4B72-9789-ADAB2969549A}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{3D37A289-CCF1-4021-9A8B-38A18056DCC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>